<commit_message>
add live_parse to classes_opt
</commit_message>
<xml_diff>
--- a/df_general.xlsx
+++ b/df_general.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="303">
   <si>
     <t>GAME_ID</t>
   </si>
@@ -658,6 +658,12 @@
     <t>Астерас Триполис</t>
   </si>
   <si>
+    <t>Антверпен</t>
+  </si>
+  <si>
+    <t>Эшторил</t>
+  </si>
+  <si>
     <t>Атлетико Мадрид</t>
   </si>
   <si>
@@ -751,9 +757,6 @@
     <t>Осасуна</t>
   </si>
   <si>
-    <t>Антверпен</t>
-  </si>
-  <si>
     <t>ОФИ</t>
   </si>
   <si>
@@ -815,9 +818,6 @@
   </si>
   <si>
     <t>Бернли</t>
-  </si>
-  <si>
-    <t>Эшторил</t>
   </si>
   <si>
     <t>Аполлон Смирна</t>
@@ -1284,7 +1284,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U229"/>
+  <dimension ref="A1:U243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1679,7 +1679,7 @@
         <v>61</v>
       </c>
       <c r="G7" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="H7" t="s">
         <v>273</v>
@@ -1809,7 +1809,7 @@
         <v>63</v>
       </c>
       <c r="G9" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H9" t="s">
         <v>270</v>
@@ -2069,7 +2069,7 @@
         <v>67</v>
       </c>
       <c r="G13" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="H13" t="s">
         <v>275</v>
@@ -2201,7 +2201,7 @@
         <v>67</v>
       </c>
       <c r="G16" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="H16" t="s">
         <v>275</v>
@@ -2398,7 +2398,7 @@
         <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H20" t="s">
         <v>274</v>
@@ -2463,7 +2463,7 @@
         <v>72</v>
       </c>
       <c r="G21" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H21" t="s">
         <v>276</v>
@@ -2593,7 +2593,7 @@
         <v>74</v>
       </c>
       <c r="G23" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H23" t="s">
         <v>269</v>
@@ -2658,7 +2658,7 @@
         <v>75</v>
       </c>
       <c r="G24" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="H24" t="s">
         <v>270</v>
@@ -2788,7 +2788,7 @@
         <v>77</v>
       </c>
       <c r="G26" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="H26" t="s">
         <v>279</v>
@@ -2853,7 +2853,7 @@
         <v>78</v>
       </c>
       <c r="G27" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="H27" t="s">
         <v>276</v>
@@ -2983,7 +2983,7 @@
         <v>80</v>
       </c>
       <c r="G29" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="H29" t="s">
         <v>275</v>
@@ -3048,7 +3048,7 @@
         <v>81</v>
       </c>
       <c r="G30" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="H30" t="s">
         <v>281</v>
@@ -3301,7 +3301,7 @@
         <v>86</v>
       </c>
       <c r="G35" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="H35" t="s">
         <v>279</v>
@@ -3366,7 +3366,7 @@
         <v>87</v>
       </c>
       <c r="G36" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="H36" t="s">
         <v>281</v>
@@ -3431,7 +3431,7 @@
         <v>88</v>
       </c>
       <c r="G37" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H37" t="s">
         <v>279</v>
@@ -3496,7 +3496,7 @@
         <v>89</v>
       </c>
       <c r="G38" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="H38" t="s">
         <v>276</v>
@@ -3691,7 +3691,7 @@
         <v>92</v>
       </c>
       <c r="G41" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="H41" t="s">
         <v>284</v>
@@ -3756,7 +3756,7 @@
         <v>93</v>
       </c>
       <c r="G42" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H42" t="s">
         <v>284</v>
@@ -4016,7 +4016,7 @@
         <v>97</v>
       </c>
       <c r="G46" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="H46" t="s">
         <v>285</v>
@@ -4146,7 +4146,7 @@
         <v>99</v>
       </c>
       <c r="G48" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="H48" t="s">
         <v>277</v>
@@ -4211,7 +4211,7 @@
         <v>100</v>
       </c>
       <c r="G49" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="H49" t="s">
         <v>279</v>
@@ -4341,7 +4341,7 @@
         <v>101</v>
       </c>
       <c r="G51" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="H51" t="s">
         <v>287</v>
@@ -4406,7 +4406,7 @@
         <v>102</v>
       </c>
       <c r="G52" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="H52" t="s">
         <v>280</v>
@@ -4471,7 +4471,7 @@
         <v>103</v>
       </c>
       <c r="G53" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="H53" t="s">
         <v>283</v>
@@ -4536,7 +4536,7 @@
         <v>104</v>
       </c>
       <c r="G54" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="H54" t="s">
         <v>279</v>
@@ -4760,7 +4760,7 @@
         <v>108</v>
       </c>
       <c r="G58" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H58" t="s">
         <v>289</v>
@@ -4816,7 +4816,7 @@
         <v>109</v>
       </c>
       <c r="G59" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H59" t="s">
         <v>289</v>
@@ -4993,7 +4993,7 @@
         <v>112</v>
       </c>
       <c r="G62" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="H62" t="s">
         <v>283</v>
@@ -5152,7 +5152,7 @@
         <v>109</v>
       </c>
       <c r="G65" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H65" t="s">
         <v>273</v>
@@ -5217,7 +5217,7 @@
         <v>108</v>
       </c>
       <c r="G66" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H66" t="s">
         <v>282</v>
@@ -5412,7 +5412,7 @@
         <v>113</v>
       </c>
       <c r="G69" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="H69" t="s">
         <v>288</v>
@@ -5542,7 +5542,7 @@
         <v>115</v>
       </c>
       <c r="G71" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="H71" t="s">
         <v>270</v>
@@ -5802,7 +5802,7 @@
         <v>119</v>
       </c>
       <c r="G75" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="H75" t="s">
         <v>270</v>
@@ -5867,7 +5867,7 @@
         <v>120</v>
       </c>
       <c r="G76" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="H76" t="s">
         <v>291</v>
@@ -5932,7 +5932,7 @@
         <v>121</v>
       </c>
       <c r="G77" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H77" t="s">
         <v>270</v>
@@ -6127,7 +6127,7 @@
         <v>69</v>
       </c>
       <c r="G80" t="s">
-        <v>245</v>
+        <v>214</v>
       </c>
       <c r="H80" t="s">
         <v>275</v>
@@ -6322,7 +6322,7 @@
         <v>126</v>
       </c>
       <c r="G83" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H83" t="s">
         <v>272</v>
@@ -6387,7 +6387,7 @@
         <v>127</v>
       </c>
       <c r="G84" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H84" t="s">
         <v>270</v>
@@ -6452,7 +6452,7 @@
         <v>128</v>
       </c>
       <c r="G85" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H85" t="s">
         <v>292</v>
@@ -6517,7 +6517,7 @@
         <v>126</v>
       </c>
       <c r="G86" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="H86" t="s">
         <v>272</v>
@@ -6582,7 +6582,7 @@
         <v>127</v>
       </c>
       <c r="G87" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="H87" t="s">
         <v>270</v>
@@ -6647,7 +6647,7 @@
         <v>128</v>
       </c>
       <c r="G88" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H88" t="s">
         <v>292</v>
@@ -7725,7 +7725,7 @@
         <v>144</v>
       </c>
       <c r="G105" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="H105" t="s">
         <v>288</v>
@@ -7790,7 +7790,7 @@
         <v>145</v>
       </c>
       <c r="G106" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="H106" t="s">
         <v>283</v>
@@ -7855,7 +7855,7 @@
         <v>99</v>
       </c>
       <c r="G107" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="H107" t="s">
         <v>275</v>
@@ -7920,7 +7920,7 @@
         <v>146</v>
       </c>
       <c r="G108" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H108" t="s">
         <v>272</v>
@@ -8310,7 +8310,7 @@
         <v>152</v>
       </c>
       <c r="G114" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H114" t="s">
         <v>275</v>
@@ -8505,7 +8505,7 @@
         <v>155</v>
       </c>
       <c r="G117" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H117" t="s">
         <v>283</v>
@@ -8570,7 +8570,7 @@
         <v>156</v>
       </c>
       <c r="G118" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="H118" t="s">
         <v>275</v>
@@ -8700,7 +8700,7 @@
         <v>158</v>
       </c>
       <c r="G120" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H120" t="s">
         <v>295</v>
@@ -8765,7 +8765,7 @@
         <v>159</v>
       </c>
       <c r="G121" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H121" t="s">
         <v>275</v>
@@ -8895,7 +8895,7 @@
         <v>161</v>
       </c>
       <c r="G123" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H123" t="s">
         <v>283</v>
@@ -9090,7 +9090,7 @@
         <v>164</v>
       </c>
       <c r="G126" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H126" t="s">
         <v>273</v>
@@ -9799,7 +9799,7 @@
         <v>169</v>
       </c>
       <c r="G137" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="H137" t="s">
         <v>283</v>
@@ -9864,7 +9864,7 @@
         <v>170</v>
       </c>
       <c r="G138" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="H138" t="s">
         <v>283</v>
@@ -9994,7 +9994,7 @@
         <v>172</v>
       </c>
       <c r="G140" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H140" t="s">
         <v>283</v>
@@ -10570,7 +10570,7 @@
         <v>178</v>
       </c>
       <c r="G149" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H149" t="s">
         <v>273</v>
@@ -10830,7 +10830,7 @@
         <v>182</v>
       </c>
       <c r="G153" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H153" t="s">
         <v>288</v>
@@ -10960,7 +10960,7 @@
         <v>184</v>
       </c>
       <c r="G155" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="H155" t="s">
         <v>275</v>
@@ -11545,7 +11545,7 @@
         <v>192</v>
       </c>
       <c r="G164" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="H164" t="s">
         <v>282</v>
@@ -11843,7 +11843,7 @@
         <v>124</v>
       </c>
       <c r="G169" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="H169" t="s">
         <v>279</v>
@@ -11908,7 +11908,7 @@
         <v>58</v>
       </c>
       <c r="G170" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="J170">
         <v>2.05</v>
@@ -12032,7 +12032,7 @@
         <v>152</v>
       </c>
       <c r="G172" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H172" t="s">
         <v>275</v>
@@ -12357,7 +12357,7 @@
         <v>197</v>
       </c>
       <c r="G177" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H177" t="s">
         <v>298</v>
@@ -12880,7 +12880,7 @@
         <v>127</v>
       </c>
       <c r="G188" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="H188" t="s">
         <v>289</v>
@@ -12936,7 +12936,7 @@
         <v>145</v>
       </c>
       <c r="G189" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H189" t="s">
         <v>279</v>
@@ -13225,7 +13225,7 @@
         <v>99</v>
       </c>
       <c r="G194" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="H194" t="s">
         <v>275</v>
@@ -13355,7 +13355,7 @@
         <v>201</v>
       </c>
       <c r="G196" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H196" t="s">
         <v>283</v>
@@ -13420,7 +13420,7 @@
         <v>158</v>
       </c>
       <c r="G197" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="H197" t="s">
         <v>299</v>
@@ -13680,7 +13680,7 @@
         <v>203</v>
       </c>
       <c r="G201" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="H201" t="s">
         <v>289</v>
@@ -13940,7 +13940,7 @@
         <v>205</v>
       </c>
       <c r="G205" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H205" t="s">
         <v>273</v>
@@ -14070,7 +14070,7 @@
         <v>61</v>
       </c>
       <c r="G207" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="H207" t="s">
         <v>282</v>
@@ -14259,7 +14259,7 @@
         <v>208</v>
       </c>
       <c r="G210" t="s">
-        <v>267</v>
+        <v>215</v>
       </c>
       <c r="H210" t="s">
         <v>276</v>
@@ -14827,7 +14827,7 @@
         <v>60</v>
       </c>
       <c r="G224" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H224" t="s">
         <v>269</v>
@@ -14856,7 +14856,7 @@
         <v>125</v>
       </c>
       <c r="G225" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H225" t="s">
         <v>289</v>
@@ -15009,6 +15009,427 @@
       </c>
       <c r="U229">
         <v>9.5</v>
+      </c>
+    </row>
+    <row r="230" spans="1:21">
+      <c r="A230" s="1">
+        <v>228</v>
+      </c>
+      <c r="B230">
+        <v>228</v>
+      </c>
+      <c r="C230" t="s">
+        <v>21</v>
+      </c>
+      <c r="D230" t="s">
+        <v>35</v>
+      </c>
+      <c r="E230" s="2">
+        <v>44586.86458333334</v>
+      </c>
+      <c r="F230" t="s">
+        <v>214</v>
+      </c>
+      <c r="G230" t="s">
+        <v>186</v>
+      </c>
+      <c r="H230" t="s">
+        <v>275</v>
+      </c>
+      <c r="I230" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="231" spans="1:21">
+      <c r="A231" s="1">
+        <v>229</v>
+      </c>
+      <c r="B231">
+        <v>229</v>
+      </c>
+      <c r="C231" t="s">
+        <v>33</v>
+      </c>
+      <c r="D231" t="s">
+        <v>46</v>
+      </c>
+      <c r="E231" s="2">
+        <v>44586.94791666666</v>
+      </c>
+      <c r="F231" t="s">
+        <v>148</v>
+      </c>
+      <c r="G231" t="s">
+        <v>170</v>
+      </c>
+      <c r="H231" t="s">
+        <v>270</v>
+      </c>
+      <c r="I231" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="232" spans="1:21">
+      <c r="A232" s="1">
+        <v>230</v>
+      </c>
+      <c r="B232">
+        <v>230</v>
+      </c>
+      <c r="C232" t="s">
+        <v>21</v>
+      </c>
+      <c r="D232" t="s">
+        <v>35</v>
+      </c>
+      <c r="E232" s="2">
+        <v>44586.95833333334</v>
+      </c>
+      <c r="F232" t="s">
+        <v>182</v>
+      </c>
+      <c r="G232" t="s">
+        <v>223</v>
+      </c>
+      <c r="H232" t="s">
+        <v>275</v>
+      </c>
+      <c r="I232" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="233" spans="1:21">
+      <c r="A233" s="1">
+        <v>231</v>
+      </c>
+      <c r="B233">
+        <v>231</v>
+      </c>
+      <c r="C233" t="s">
+        <v>21</v>
+      </c>
+      <c r="D233" t="s">
+        <v>35</v>
+      </c>
+      <c r="E233" s="2">
+        <v>44586.95833333334</v>
+      </c>
+      <c r="F233" t="s">
+        <v>57</v>
+      </c>
+      <c r="G233" t="s">
+        <v>179</v>
+      </c>
+      <c r="H233" t="s">
+        <v>275</v>
+      </c>
+      <c r="I233" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="234" spans="1:21">
+      <c r="A234" s="1">
+        <v>232</v>
+      </c>
+      <c r="B234">
+        <v>232</v>
+      </c>
+      <c r="C234" t="s">
+        <v>33</v>
+      </c>
+      <c r="D234" t="s">
+        <v>46</v>
+      </c>
+      <c r="E234" s="2">
+        <v>44587.94791666666</v>
+      </c>
+      <c r="F234" t="s">
+        <v>172</v>
+      </c>
+      <c r="G234" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="235" spans="1:21">
+      <c r="A235" s="1">
+        <v>233</v>
+      </c>
+      <c r="B235">
+        <v>233</v>
+      </c>
+      <c r="C235" t="s">
+        <v>33</v>
+      </c>
+      <c r="D235" t="s">
+        <v>46</v>
+      </c>
+      <c r="E235" s="2">
+        <v>44587.94791666666</v>
+      </c>
+      <c r="F235" t="s">
+        <v>146</v>
+      </c>
+      <c r="G235" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="236" spans="1:21">
+      <c r="A236" s="1">
+        <v>234</v>
+      </c>
+      <c r="B236">
+        <v>234</v>
+      </c>
+      <c r="C236" t="s">
+        <v>33</v>
+      </c>
+      <c r="D236" t="s">
+        <v>46</v>
+      </c>
+      <c r="E236" s="2">
+        <v>44587.94791666666</v>
+      </c>
+      <c r="F236" t="s">
+        <v>169</v>
+      </c>
+      <c r="G236" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="237" spans="1:21">
+      <c r="A237" s="1">
+        <v>235</v>
+      </c>
+      <c r="B237">
+        <v>235</v>
+      </c>
+      <c r="C237" t="s">
+        <v>33</v>
+      </c>
+      <c r="D237" t="s">
+        <v>46</v>
+      </c>
+      <c r="E237" s="2">
+        <v>44587.94791666666</v>
+      </c>
+      <c r="F237" t="s">
+        <v>176</v>
+      </c>
+      <c r="G237" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="238" spans="1:21">
+      <c r="A238" s="1">
+        <v>236</v>
+      </c>
+      <c r="B238">
+        <v>236</v>
+      </c>
+      <c r="C238" t="s">
+        <v>33</v>
+      </c>
+      <c r="D238" t="s">
+        <v>46</v>
+      </c>
+      <c r="E238" s="2">
+        <v>44587.94791666666</v>
+      </c>
+      <c r="F238" t="s">
+        <v>171</v>
+      </c>
+      <c r="G238" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="239" spans="1:21">
+      <c r="A239" s="1">
+        <v>237</v>
+      </c>
+      <c r="B239">
+        <v>237</v>
+      </c>
+      <c r="C239" t="s">
+        <v>21</v>
+      </c>
+      <c r="D239" t="s">
+        <v>35</v>
+      </c>
+      <c r="E239" s="2">
+        <v>44588.94791666666</v>
+      </c>
+      <c r="F239" t="s">
+        <v>62</v>
+      </c>
+      <c r="G239" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="240" spans="1:21">
+      <c r="A240" s="1">
+        <v>238</v>
+      </c>
+      <c r="B240">
+        <v>238</v>
+      </c>
+      <c r="C240" t="s">
+        <v>22</v>
+      </c>
+      <c r="D240" t="s">
+        <v>36</v>
+      </c>
+      <c r="E240" s="2">
+        <v>44588.96875</v>
+      </c>
+      <c r="F240" t="s">
+        <v>215</v>
+      </c>
+      <c r="G240" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="241" spans="1:21">
+      <c r="A241" s="1">
+        <v>239</v>
+      </c>
+      <c r="B241">
+        <v>239</v>
+      </c>
+      <c r="C241" t="s">
+        <v>21</v>
+      </c>
+      <c r="D241" t="s">
+        <v>35</v>
+      </c>
+      <c r="E241" s="2">
+        <v>44588.94791666666</v>
+      </c>
+      <c r="F241" t="s">
+        <v>62</v>
+      </c>
+      <c r="G241" t="s">
+        <v>94</v>
+      </c>
+      <c r="H241" t="s">
+        <v>289</v>
+      </c>
+      <c r="I241" t="s">
+        <v>302</v>
+      </c>
+      <c r="J241">
+        <v>2.23</v>
+      </c>
+      <c r="K241">
+        <v>3.8</v>
+      </c>
+      <c r="L241">
+        <v>2.95</v>
+      </c>
+      <c r="M241">
+        <v>2.26</v>
+      </c>
+      <c r="N241">
+        <v>3.8</v>
+      </c>
+      <c r="O241">
+        <v>2.9</v>
+      </c>
+      <c r="P241">
+        <v>2.31</v>
+      </c>
+      <c r="Q241">
+        <v>3.7</v>
+      </c>
+      <c r="R241">
+        <v>2.85</v>
+      </c>
+      <c r="S241">
+        <v>2.28</v>
+      </c>
+      <c r="T241">
+        <v>3.65</v>
+      </c>
+      <c r="U241">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="242" spans="1:21">
+      <c r="A242" s="1">
+        <v>240</v>
+      </c>
+      <c r="B242">
+        <v>240</v>
+      </c>
+      <c r="C242" t="s">
+        <v>22</v>
+      </c>
+      <c r="D242" t="s">
+        <v>36</v>
+      </c>
+      <c r="E242" s="2">
+        <v>44588.96875</v>
+      </c>
+      <c r="F242" t="s">
+        <v>215</v>
+      </c>
+      <c r="G242" t="s">
+        <v>66</v>
+      </c>
+      <c r="H242" t="s">
+        <v>272</v>
+      </c>
+      <c r="I242" t="s">
+        <v>301</v>
+      </c>
+      <c r="J242">
+        <v>1.98</v>
+      </c>
+      <c r="K242">
+        <v>3.25</v>
+      </c>
+      <c r="L242">
+        <v>4.1</v>
+      </c>
+      <c r="M242">
+        <v>1.98</v>
+      </c>
+      <c r="N242">
+        <v>3.25</v>
+      </c>
+      <c r="O242">
+        <v>4.1</v>
+      </c>
+      <c r="P242">
+        <v>2</v>
+      </c>
+      <c r="Q242">
+        <v>3.2</v>
+      </c>
+      <c r="R242">
+        <v>4.1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:21">
+      <c r="A243" s="1">
+        <v>241</v>
+      </c>
+      <c r="B243">
+        <v>241</v>
+      </c>
+      <c r="C243" t="s">
+        <v>21</v>
+      </c>
+      <c r="D243" t="s">
+        <v>35</v>
+      </c>
+      <c r="E243" s="2">
+        <v>44589.94791666666</v>
+      </c>
+      <c r="F243" t="s">
+        <v>186</v>
+      </c>
+      <c r="G243" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>